<commit_message>
problem found and results tracking
</commit_message>
<xml_diff>
--- a/tryingInterp3/2015-1-1.xlsx
+++ b/tryingInterp3/2015-1-1.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
   <si>
     <t>interpolation</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,23 +54,391 @@
   <si>
     <t>8,8,4</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> c1 = 4;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> c2 = 4;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> c3 = 4;</t>
+  </si>
+  <si>
+    <t>Smax = 4; Smin = 0*S0;</t>
+  </si>
+  <si>
+    <t>vmax = 0.25; vmin = 0;</t>
+  </si>
+  <si>
+    <t>rmax = 0.1; rmin = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 1.267031e+03 s </t>
+  </si>
+  <si>
+    <t>Time: 40 ;Iterations: 6</t>
+  </si>
+  <si>
+    <t>Time: 80 ;Iterations: 5</t>
+  </si>
+  <si>
+    <t>Time: 120 ;Iterations: 5</t>
+  </si>
+  <si>
+    <t>Time: 160 ;Iterations: 5</t>
+  </si>
+  <si>
+    <t>Time: 200 ;Iterations: 5</t>
+  </si>
+  <si>
+    <t>levels:  5  0  0, grid size: 129 * 5 * 5 = 3225</t>
+  </si>
+  <si>
+    <t>Stock price: 1.1000 Variance: 0.04 Interest: 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The calculated option price is 0.024786 </t>
+  </si>
+  <si>
+    <t>run time: 19.808784 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                </t>
+  </si>
+  <si>
+    <r>
+      <t>[esti,details]=MainFunc(3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,1.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 1.289938e+03 s </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> [esti,details]=MainFunc(3,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Benchmark  : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2.461800 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The estimated American Mother Option price: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.445661</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The estimated American Mother Option price: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.183599</t>
+    </r>
+  </si>
+  <si>
+    <t>Stock price: 1.2000 Variance: 0.04 Interest: 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The calculated option price is 0.013466 </t>
+  </si>
+  <si>
+    <t>run time: 19.836193 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benchmark  : 1.177400 </t>
+  </si>
+  <si>
+    <t>Stock price: 1.0000 Variance: 0.04 Interest: 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The calculated option price is 0.043296 </t>
+  </si>
+  <si>
+    <t>run time: 23.955807 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 1.700891e+03 s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benchmark  : 5.022700 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The estimated American Mother Option price: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5.079859</t>
+    </r>
+  </si>
+  <si>
+    <t>matrix K,A completed, run time: 27.114552 s</t>
+  </si>
+  <si>
+    <t>matrix K,A completed, run time: 27.463668 s</t>
+  </si>
+  <si>
+    <r>
+      <t>[esti,details]=MainFunc(3,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>Stock price: 0.9000 Variance: 0.04 Interest: 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The calculated option price is 0.094204 </t>
+  </si>
+  <si>
+    <t>run time: 19.891089 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 1.284328e+03 s </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The estimated American Mother Option price: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9.603585</t>
+    </r>
+  </si>
+  <si>
+    <t>Benchmark  : 9.685600</t>
+  </si>
+  <si>
+    <r>
+      <t>[esti,details]=MainFunc(3,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>matrix K,A completed, run time: 27.355995 s</t>
+  </si>
+  <si>
+    <t>Stock price: 0.8000 Variance: 0.04 Interest: 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The calculated option price is 0.171893 </t>
+  </si>
+  <si>
+    <t>run time: 20.222632 seconds</t>
+  </si>
+  <si>
+    <t>matrix K,A completed, run time: 27.873963 s</t>
+  </si>
+  <si>
+    <r>
+      <t>[esti,details]=MainFunc(3,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 1.275516e+03 s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benchmark  : 16.951200 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The estimated American Mother Option price: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>17.020193</t>
+    </r>
+  </si>
+  <si>
+    <t>matrix K,A completed, run time: 26.672999 s</t>
+  </si>
+  <si>
+    <t>The estimated American Mother Option price: 17.249787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 1.272578e+03 s </t>
+  </si>
+  <si>
+    <t>Smax = 8; Smin = 0*S0;</t>
+  </si>
+  <si>
+    <t>vmax = 0.5; vmin = 0;</t>
+  </si>
+  <si>
+    <t>rmax = 0.25; rmin = 0;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -77,14 +446,28 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -97,7 +480,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -105,14 +488,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -419,21 +892,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -453,12 +926,12 @@
         <v>1.1774</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -478,7 +951,7 @@
         <v>0.57089999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -498,7 +971,7 @@
         <v>0.82509999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -509,17 +982,17 @@
         <v>17.007400000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="F9">
         <v>0.82504999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="F10">
         <v>1.02319</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -539,7 +1012,7 @@
         <v>1.0166999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -547,7 +1020,7 @@
         <v>4.6670999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -561,12 +1034,12 @@
         <v>0.65139999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -591,4 +1064,713 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="6" max="6" width="3.109375" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" customWidth="1"/>
+    <col min="19" max="19" width="3.109375" customWidth="1"/>
+    <col min="24" max="24" width="11.5546875" customWidth="1"/>
+    <col min="26" max="26" width="3" customWidth="1"/>
+    <col min="33" max="33" width="5.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="H5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="5"/>
+      <c r="N5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="5"/>
+      <c r="U5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="5"/>
+      <c r="AB5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="5"/>
+    </row>
+    <row r="6" spans="1:33">
+      <c r="A6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="H6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="8"/>
+      <c r="N6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="U6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="8"/>
+      <c r="AB6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="8"/>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="H7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="8"/>
+      <c r="N7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="8"/>
+      <c r="U7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="8"/>
+      <c r="AB7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="8"/>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="H8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="8"/>
+      <c r="N8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="8"/>
+      <c r="U8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="8"/>
+      <c r="AB8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="8"/>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="H9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="8"/>
+      <c r="N9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="U9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="8"/>
+      <c r="AB9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="8"/>
+    </row>
+    <row r="10" spans="1:33">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="H10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="8"/>
+      <c r="N10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="8"/>
+      <c r="U10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="8"/>
+      <c r="AB10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="8"/>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+      <c r="H11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="8"/>
+      <c r="N11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="8"/>
+      <c r="U11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="8"/>
+      <c r="AB11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="8"/>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="H12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="N12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="8"/>
+      <c r="U12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="8"/>
+      <c r="AB12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="8"/>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="H13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="8"/>
+      <c r="N13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="8"/>
+      <c r="U13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="8"/>
+      <c r="AB13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="8"/>
+    </row>
+    <row r="14" spans="1:33">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="H14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="8"/>
+      <c r="N14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="8"/>
+      <c r="U14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="8"/>
+      <c r="AB14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="8"/>
+    </row>
+    <row r="15" spans="1:33">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="H15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="8"/>
+      <c r="N15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="8"/>
+      <c r="U15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="8"/>
+      <c r="AB15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="8"/>
+    </row>
+    <row r="16" spans="1:33">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="8"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="8"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="8"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="8"/>
+    </row>
+    <row r="17" spans="1:33">
+      <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="H17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="8"/>
+      <c r="N17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="8"/>
+      <c r="U17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="8"/>
+      <c r="AB17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="8"/>
+    </row>
+    <row r="18" spans="1:33">
+      <c r="A18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L18" s="8"/>
+      <c r="N18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="R18" s="7"/>
+      <c r="S18" s="8"/>
+      <c r="U18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="8"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="8"/>
+    </row>
+    <row r="19" spans="1:33">
+      <c r="A19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="H19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+      <c r="N19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="11"/>
+      <c r="U19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="11"/>
+      <c r="AB19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="11"/>
+    </row>
+    <row r="21" spans="1:33">
+      <c r="X21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
+      <c r="AG21" s="5"/>
+    </row>
+    <row r="22" spans="1:33">
+      <c r="X22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
+      <c r="AB22" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC22" s="7"/>
+      <c r="AD22" s="7"/>
+      <c r="AE22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF22" s="7"/>
+      <c r="AG22" s="8"/>
+    </row>
+    <row r="23" spans="1:33">
+      <c r="X23" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC23" s="10"/>
+      <c r="AD23" s="10"/>
+      <c r="AE23" s="10"/>
+      <c r="AF23" s="10"/>
+      <c r="AG23" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Some ressults of interpolation involved
16,8,4 interpolation results
</commit_message>
<xml_diff>
--- a/tryingInterp3/2015-1-1.xlsx
+++ b/tryingInterp3/2015-1-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
   <si>
     <t>interpolation</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -422,6 +422,54 @@
   </si>
   <si>
     <t>rmax = 0.25; rmin = 0;</t>
+  </si>
+  <si>
+    <t>The estimated American Mother Option price: 17.108034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                              Benchmark   : 16.951200 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 1.264438e+03 s </t>
+  </si>
+  <si>
+    <t>cubic</t>
+  </si>
+  <si>
+    <t>The estimated American Mother Option price: 17.007496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 4.196047e+03 s </t>
+  </si>
+  <si>
+    <t>level=4</t>
+  </si>
+  <si>
+    <t>The estimated American Mother Option price: 9.403362</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                              Benchmark   : 9.685600 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 2.778828e+03 s </t>
+  </si>
+  <si>
+    <t>The estimated American Mother Option price: 1.127158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                              Benchmark   : 1.177400 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 1.290547e+03 s </t>
+  </si>
+  <si>
+    <t>The estimated American Mother Option price: 2.561558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                              Benchmark   : 2.461800 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Total time spent: 1.267109e+03 s </t>
   </si>
 </sst>
 </file>
@@ -572,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -586,6 +634,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1068,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG23"/>
+  <dimension ref="A1:AG30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1719,7 +1769,15 @@
       <c r="AF19" s="10"/>
       <c r="AG19" s="11"/>
     </row>
+    <row r="20" spans="1:33">
+      <c r="A20" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="21" spans="1:33">
+      <c r="A21" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="X21" s="3" t="s">
         <v>66</v>
       </c>
@@ -1736,6 +1794,9 @@
       <c r="AG21" s="5"/>
     </row>
     <row r="22" spans="1:33">
+      <c r="A22" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="X22" s="6" t="s">
         <v>67</v>
       </c>
@@ -1754,6 +1815,9 @@
       <c r="AG22" s="8"/>
     </row>
     <row r="23" spans="1:33">
+      <c r="A23" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="X23" s="9" t="s">
         <v>68</v>
       </c>
@@ -1769,6 +1833,124 @@
       <c r="AF23" s="10"/>
       <c r="AG23" s="11"/>
     </row>
+    <row r="24" spans="1:33">
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="4"/>
+      <c r="AG24" s="5"/>
+    </row>
+    <row r="25" spans="1:33">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" t="s">
+        <v>79</v>
+      </c>
+      <c r="U25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="5"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="4"/>
+      <c r="AF25" s="4"/>
+      <c r="AG25" s="5"/>
+    </row>
+    <row r="26" spans="1:33">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" t="s">
+        <v>80</v>
+      </c>
+      <c r="U26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="8"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC26" s="7"/>
+      <c r="AD26" s="7"/>
+      <c r="AE26" s="7"/>
+      <c r="AF26" s="7"/>
+      <c r="AG26" s="8"/>
+    </row>
+    <row r="27" spans="1:33">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" t="s">
+        <v>81</v>
+      </c>
+      <c r="U27" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="11"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC27" s="10"/>
+      <c r="AD27" s="10"/>
+      <c r="AE27" s="10"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="11"/>
+    </row>
+    <row r="28" spans="1:33">
+      <c r="AA28" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="4"/>
+      <c r="AF28" s="4"/>
+      <c r="AG28" s="5"/>
+    </row>
+    <row r="29" spans="1:33">
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC29" s="7"/>
+      <c r="AD29" s="7"/>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="7"/>
+      <c r="AG29" s="8"/>
+    </row>
+    <row r="30" spans="1:33">
+      <c r="AA30" s="9"/>
+      <c r="AB30" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC30" s="10"/>
+      <c r="AD30" s="10"/>
+      <c r="AE30" s="10"/>
+      <c r="AF30" s="10"/>
+      <c r="AG30" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>